<commit_message>
class 32 and 34
</commit_message>
<xml_diff>
--- a/testdata/Excel.xlsx
+++ b/testdata/Excel.xlsx
@@ -4,17 +4,17 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="25200" windowHeight="12131"/>
+    <workbookView windowWidth="23040" windowHeight="9335"/>
   </bookViews>
   <sheets>
-    <sheet name="Excel" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
   <si>
     <t>FirstName</t>
   </si>
@@ -42,14 +42,20 @@
   <si>
     <t>Ann</t>
   </si>
+  <si>
+    <t>Ali</t>
+  </si>
+  <si>
+    <t>Tarlaci</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
@@ -63,21 +69,22 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -98,21 +105,45 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -121,6 +152,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
@@ -128,9 +167,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -145,7 +191,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -155,14 +201,6 @@
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -173,38 +211,6 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -215,6 +221,174 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -227,175 +401,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -406,6 +412,21 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -445,16 +466,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -470,21 +491,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -508,18 +514,16 @@
     </border>
   </borders>
   <cellStyleXfs count="49">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -529,140 +533,136 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="23" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="16" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -725,7 +725,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -982,15 +982,15 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10" defaultRowHeight="14.4" outlineLevelRow="2" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="3" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="16384" width="10" style="1"/>
+    <col min="1" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1015,7 +1015,7 @@
         <v>5</v>
       </c>
       <c r="C2" s="1">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>6</v>
@@ -1035,8 +1035,22 @@
         <v>6</v>
       </c>
     </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="1">
+        <v>28</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
 </worksheet>
 </file>
</xml_diff>